<commit_message>
added login and cart functions
</commit_message>
<xml_diff>
--- a/ecommerce/configs/data.xlsx
+++ b/ecommerce/configs/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="registration" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="login" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="registration" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="login" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -634,7 +634,7 @@
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -733,7 +733,7 @@
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="G12" s="3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
     </row>

</xml_diff>